<commit_message>
Snake display and movement
</commit_message>
<xml_diff>
--- a/Conception/Planification.xlsx
+++ b/Conception/Planification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_SnA.I.ke\Conception\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54FD7F29-9023-4547-82B0-E370C836BE9E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B3F3E4-533F-42C3-AEC5-4E4C58A34FC5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="1" xr2:uid="{35E463D2-E3B9-4A49-AEC3-8C78D61E9D3F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{35E463D2-E3B9-4A49-AEC3-8C78D61E9D3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Planif" sheetId="1" r:id="rId1"/>
@@ -201,7 +201,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="50">
   <si>
     <t>François Thérien</t>
   </si>
@@ -348,13 +348,16 @@
   </si>
   <si>
     <t>Difficulté * Temps(min)</t>
+  </si>
+  <si>
+    <t>Est fait</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -397,8 +400,15 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -414,6 +424,11 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
       </patternFill>
     </fill>
   </fills>
@@ -486,13 +501,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -507,9 +523,16 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="40 % - Accent1" xfId="3" builtinId="31"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
     <cellStyle name="Calcul" xfId="2" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Sortie" xfId="1" builtinId="21"/>
@@ -880,10 +903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14BBF500-7C10-41A0-AE8D-140DD1F019B0}">
-  <dimension ref="B4:R26"/>
+  <dimension ref="B4:T26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T22" sqref="T22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,19 +922,24 @@
     <col min="17" max="17" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:18" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:20" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="G4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:18" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="T6" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20" ht="23.25" x14ac:dyDescent="0.35">
       <c r="M7" s="2"/>
       <c r="N7" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="K8" s="3" t="s">
         <v>2</v>
       </c>
@@ -937,55 +965,55 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="K9" s="4">
-        <v>1</v>
-      </c>
-      <c r="L9" s="5" t="s">
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="K9" s="10">
+        <v>1</v>
+      </c>
+      <c r="L9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="5"/>
-      <c r="N9" s="6" t="s">
+      <c r="M9" s="11"/>
+      <c r="N9" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="O9" s="6" t="s">
+      <c r="O9" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="P9" s="6" t="s">
+      <c r="P9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="Q9" s="5">
+      <c r="Q9" s="11">
         <v>30</v>
       </c>
-      <c r="R9" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="K10" s="4">
+      <c r="R9" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="K10" s="10">
         <v>2</v>
       </c>
-      <c r="L10" s="5" t="s">
+      <c r="L10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="M10" s="5"/>
-      <c r="N10" s="6" t="s">
+      <c r="M10" s="11"/>
+      <c r="N10" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="O10" s="6" t="s">
+      <c r="O10" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="P10" s="6" t="s">
+      <c r="P10" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="Q10" s="5">
+      <c r="Q10" s="11">
         <v>180</v>
       </c>
-      <c r="R10" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R10" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="K11" s="4">
         <v>3</v>
       </c>
@@ -1009,7 +1037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="K12" s="4">
         <v>4</v>
       </c>
@@ -1033,7 +1061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="K13" s="4">
         <v>5</v>
       </c>
@@ -1057,7 +1085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="K14" s="4">
         <v>6</v>
       </c>
@@ -1081,7 +1109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="K15" s="4">
         <v>7</v>
       </c>
@@ -1105,7 +1133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="K16" s="4">
         <v>8</v>
       </c>
@@ -1380,7 +1408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784D2701-793A-4653-90AF-774ED7622AEF}">
   <dimension ref="G6:S24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added saving and loading already trained qNetwork
</commit_message>
<xml_diff>
--- a/Conception/Planification.xlsx
+++ b/Conception/Planification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_SnA.I.ke\Conception\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D96FAA-4DE7-4A3D-B4AF-7659BE6640F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C420EC-9E2B-4A88-8BA3-828738A26CDA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{35E463D2-E3B9-4A49-AEC3-8C78D61E9D3F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{35E463D2-E3B9-4A49-AEC3-8C78D61E9D3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Planif" sheetId="1" r:id="rId1"/>
@@ -46,8 +46,11 @@
     <author>tc={B076E583-36DE-4E57-B228-8C54754A1AAD}</author>
     <author>tc={85BDD56E-4035-4135-9DF2-4DD79ABCB301}</author>
     <author>tc={E6777460-6C19-4130-A278-25DF86D67405}</author>
+    <author>tc={92FF6DDF-727B-4F55-A7E9-F4A5D0223FC8}</author>
     <author>tc={1521FCB4-2E5C-41EB-BD4A-CA08A349950D}</author>
+    <author>tc={D766CD36-CA28-4C5E-B88D-A0061F2D643E}</author>
     <author>tc={1FB4C5A2-DA49-46A3-8625-B9746D0C7F6B}</author>
+    <author>tc={D4721450-1B34-4173-8AC8-252704F05BC2}</author>
     <author>tc={E89A817C-DADD-49C5-971F-F82C83DE108B}</author>
     <author>tc={BF349A5F-5689-44A0-9BEA-E679C0006B78}</author>
     <author>tc={652950B0-8407-409A-ABF0-DD6BB8D5FD6F}</author>
@@ -126,7 +129,15 @@
     Pouvoir faire jouer une simulation DQL. On veut ici que les classes AI et les fonctionnalitées du jeu soient reliées afin que l'agent apprenne le jeu</t>
       </text>
     </comment>
-    <comment ref="M20" authorId="9" shapeId="0" xr:uid="{1521FCB4-2E5C-41EB-BD4A-CA08A349950D}">
+    <comment ref="T19" authorId="9" shapeId="0" xr:uid="{92FF6DDF-727B-4F55-A7E9-F4A5D0223FC8}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    Mon algorithme d'apprentissage fonctionne avec mon jeu de snake. Par contre, je ne réussi pas encore à pouvoir passer le tableau de vision du serpent à mon réseau de neurone, ne permettant pas à l'agent de bien apprendre de son environnement.</t>
+      </text>
+    </comment>
+    <comment ref="M20" authorId="10" shapeId="0" xr:uid="{1521FCB4-2E5C-41EB-BD4A-CA08A349950D}">
       <text>
         <t>[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
@@ -134,7 +145,15 @@
     Nous voulons simplement faire jouer 4 simulations en même temps</t>
       </text>
     </comment>
-    <comment ref="M21" authorId="10" shapeId="0" xr:uid="{1FB4C5A2-DA49-46A3-8625-B9746D0C7F6B}">
+    <comment ref="T20" authorId="11" shapeId="0" xr:uid="{D766CD36-CA28-4C5E-B88D-A0061F2D643E}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    J'ai besoins de l'étape  11</t>
+      </text>
+    </comment>
+    <comment ref="M21" authorId="12" shapeId="0" xr:uid="{1FB4C5A2-DA49-46A3-8625-B9746D0C7F6B}">
       <text>
         <t>[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
@@ -142,7 +161,15 @@
     Pouvoir enregistrer chaque episodes et leeurs informations pertinentes dans la bas de données</t>
       </text>
     </comment>
-    <comment ref="M22" authorId="11" shapeId="0" xr:uid="{E89A817C-DADD-49C5-971F-F82C83DE108B}">
+    <comment ref="T21" authorId="13" shapeId="0" xr:uid="{D4721450-1B34-4173-8AC8-252704F05BC2}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    J'ai besoins de l'étape 11</t>
+      </text>
+    </comment>
+    <comment ref="M22" authorId="14" shapeId="0" xr:uid="{E89A817C-DADD-49C5-971F-F82C83DE108B}">
       <text>
         <t>[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
@@ -150,7 +177,7 @@
     Pouvoir faire afficher les informations pertinentes des 4 simulations, ainsi que les fonctionnalitées de contrôle comme mettre les simulations sur pause</t>
       </text>
     </comment>
-    <comment ref="M23" authorId="12" shapeId="0" xr:uid="{BF349A5F-5689-44A0-9BEA-E679C0006B78}">
+    <comment ref="M23" authorId="15" shapeId="0" xr:uid="{BF349A5F-5689-44A0-9BEA-E679C0006B78}">
       <text>
         <t>[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
@@ -158,7 +185,7 @@
     Pouvoir ajuster les paramètres de la simulation, comme la couleur du snake ou la taille du tableau</t>
       </text>
     </comment>
-    <comment ref="M24" authorId="13" shapeId="0" xr:uid="{652950B0-8407-409A-ABF0-DD6BB8D5FD6F}">
+    <comment ref="M24" authorId="16" shapeId="0" xr:uid="{652950B0-8407-409A-ABF0-DD6BB8D5FD6F}">
       <text>
         <t>[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
@@ -166,7 +193,7 @@
     Pouvoir choisir le graphique que nous voulons consulter. Ceci implique naturellement d'aller chercher et stocker les informations nécessaire de la base de données</t>
       </text>
     </comment>
-    <comment ref="M25" authorId="14" shapeId="0" xr:uid="{183FF576-C8D6-4E20-A7B6-2E65484E1BDD}">
+    <comment ref="M25" authorId="17" shapeId="0" xr:uid="{183FF576-C8D6-4E20-A7B6-2E65484E1BDD}">
       <text>
         <t>[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
@@ -201,7 +228,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="55">
   <si>
     <t>François Thérien</t>
   </si>
@@ -357,13 +384,22 @@
   </si>
   <si>
     <t>Qnetwork et ReplayBuffer</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Raison</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -413,6 +449,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -456,7 +498,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -524,6 +566,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -535,7 +616,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -551,17 +632,34 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="6" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="6" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="4"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="4" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="4" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="3" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -917,11 +1015,20 @@
   <threadedComment ref="M19" dT="2021-03-05T19:59:54.88" personId="{75802658-D675-4BD8-B321-F64487E714A5}" id="{E6777460-6C19-4130-A278-25DF86D67405}">
     <text>Pouvoir faire jouer une simulation DQL. On veut ici que les classes AI et les fonctionnalitées du jeu soient reliées afin que l'agent apprenne le jeu</text>
   </threadedComment>
+  <threadedComment ref="T19" dT="2021-04-14T23:19:35.70" personId="{75802658-D675-4BD8-B321-F64487E714A5}" id="{92FF6DDF-727B-4F55-A7E9-F4A5D0223FC8}">
+    <text>Mon algorithme d'apprentissage fonctionne avec mon jeu de snake. Par contre, je ne réussi pas encore à pouvoir passer le tableau de vision du serpent à mon réseau de neurone, ne permettant pas à l'agent de bien apprendre de son environnement.</text>
+  </threadedComment>
   <threadedComment ref="M20" dT="2021-03-05T20:02:11.35" personId="{75802658-D675-4BD8-B321-F64487E714A5}" id="{1521FCB4-2E5C-41EB-BD4A-CA08A349950D}">
     <text>Nous voulons simplement faire jouer 4 simulations en même temps</text>
   </threadedComment>
+  <threadedComment ref="T20" dT="2021-04-14T23:54:15.30" personId="{75802658-D675-4BD8-B321-F64487E714A5}" id="{D766CD36-CA28-4C5E-B88D-A0061F2D643E}">
+    <text>J'ai besoins de l'étape  11</text>
+  </threadedComment>
   <threadedComment ref="M21" dT="2021-03-05T20:03:27.12" personId="{75802658-D675-4BD8-B321-F64487E714A5}" id="{1FB4C5A2-DA49-46A3-8625-B9746D0C7F6B}">
     <text>Pouvoir enregistrer chaque episodes et leeurs informations pertinentes dans la bas de données</text>
+  </threadedComment>
+  <threadedComment ref="T21" dT="2021-04-14T23:54:49.83" personId="{75802658-D675-4BD8-B321-F64487E714A5}" id="{D4721450-1B34-4173-8AC8-252704F05BC2}">
+    <text>J'ai besoins de l'étape 11</text>
   </threadedComment>
   <threadedComment ref="M22" dT="2021-03-05T21:23:18.92" personId="{75802658-D675-4BD8-B321-F64487E714A5}" id="{E89A817C-DADD-49C5-971F-F82C83DE108B}">
     <text>Pouvoir faire afficher les informations pertinentes des 4 simulations, ainsi que les fonctionnalitées de contrôle comme mettre les simulations sur pause</text>
@@ -943,7 +1050,7 @@
   <dimension ref="B4:V26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="U29" sqref="U29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,8 +1112,14 @@
       <c r="Q8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="R8" s="3" t="s">
+      <c r="R8" s="20" t="s">
         <v>7</v>
+      </c>
+      <c r="S8" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="T8" s="27" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
@@ -1029,8 +1142,14 @@
       <c r="Q9" s="11">
         <v>30</v>
       </c>
-      <c r="R9" s="11">
-        <v>1</v>
+      <c r="R9" s="21">
+        <v>1</v>
+      </c>
+      <c r="S9" s="28">
+        <v>1</v>
+      </c>
+      <c r="T9" s="29" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.25">
@@ -1053,8 +1172,14 @@
       <c r="Q10" s="11">
         <v>180</v>
       </c>
-      <c r="R10" s="11">
-        <v>1</v>
+      <c r="R10" s="21">
+        <v>1</v>
+      </c>
+      <c r="S10" s="28">
+        <v>1</v>
+      </c>
+      <c r="T10" s="29" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.25">
@@ -1077,8 +1202,14 @@
       <c r="Q11" s="11">
         <v>180</v>
       </c>
-      <c r="R11" s="11">
-        <v>1</v>
+      <c r="R11" s="21">
+        <v>1</v>
+      </c>
+      <c r="S11" s="28">
+        <v>1</v>
+      </c>
+      <c r="T11" s="29" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.25">
@@ -1101,8 +1232,14 @@
       <c r="Q12" s="11">
         <v>30</v>
       </c>
-      <c r="R12" s="11">
-        <v>1</v>
+      <c r="R12" s="21">
+        <v>1</v>
+      </c>
+      <c r="S12" s="28">
+        <v>1</v>
+      </c>
+      <c r="T12" s="29" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.25">
@@ -1125,8 +1262,14 @@
       <c r="Q13" s="11">
         <v>180</v>
       </c>
-      <c r="R13" s="11">
-        <v>1</v>
+      <c r="R13" s="21">
+        <v>1</v>
+      </c>
+      <c r="S13" s="28">
+        <v>1</v>
+      </c>
+      <c r="T13" s="29" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.25">
@@ -1149,59 +1292,77 @@
       <c r="Q14" s="11">
         <v>160</v>
       </c>
-      <c r="R14" s="11">
-        <v>1</v>
+      <c r="R14" s="21">
+        <v>1</v>
+      </c>
+      <c r="S14" s="28">
+        <v>1</v>
+      </c>
+      <c r="T14" s="29" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="K15" s="13">
+      <c r="K15" s="10">
         <v>7</v>
       </c>
-      <c r="L15" s="14" t="s">
+      <c r="L15" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14">
+      <c r="M15" s="11"/>
+      <c r="N15" s="11">
         <v>2</v>
       </c>
-      <c r="O15" s="15" t="s">
+      <c r="O15" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="P15" s="15" t="s">
+      <c r="P15" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="Q15" s="14">
+      <c r="Q15" s="11">
         <v>45</v>
       </c>
-      <c r="R15" s="14">
-        <v>1</v>
+      <c r="R15" s="21">
+        <v>1</v>
+      </c>
+      <c r="S15" s="28">
+        <v>1</v>
+      </c>
+      <c r="T15" s="29" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="K16" s="13">
+      <c r="K16" s="10">
         <v>8</v>
       </c>
-      <c r="L16" s="14" t="s">
+      <c r="L16" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14">
+      <c r="M16" s="11"/>
+      <c r="N16" s="11">
         <v>2</v>
       </c>
-      <c r="O16" s="15" t="s">
+      <c r="O16" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="P16" s="15" t="s">
+      <c r="P16" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="Q16" s="14">
+      <c r="Q16" s="11">
         <v>45</v>
       </c>
-      <c r="R16" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="11:18" x14ac:dyDescent="0.25">
+      <c r="R16" s="21">
+        <v>1</v>
+      </c>
+      <c r="S16" s="28">
+        <v>1</v>
+      </c>
+      <c r="T16" s="29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="11:20" x14ac:dyDescent="0.25">
       <c r="K17" s="16">
         <v>9</v>
       </c>
@@ -1221,11 +1382,17 @@
       <c r="Q17" s="16">
         <v>270</v>
       </c>
-      <c r="R17" s="16">
+      <c r="R17" s="22">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="11:18" x14ac:dyDescent="0.25">
+      <c r="S17" s="28">
+        <v>1</v>
+      </c>
+      <c r="T17" s="29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="11:20" x14ac:dyDescent="0.25">
       <c r="K18" s="16">
         <v>10</v>
       </c>
@@ -1245,200 +1412,248 @@
       <c r="Q18" s="16">
         <v>160</v>
       </c>
-      <c r="R18" s="16">
+      <c r="R18" s="22">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K19" s="16">
+      <c r="S18" s="28">
+        <v>1</v>
+      </c>
+      <c r="T18" s="29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="11:20" x14ac:dyDescent="0.25">
+      <c r="K19" s="18">
         <v>11</v>
       </c>
-      <c r="L19" s="16" t="s">
+      <c r="L19" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="M19" s="16"/>
-      <c r="N19" s="17" t="s">
+      <c r="M19" s="18"/>
+      <c r="N19" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="O19" s="17" t="s">
+      <c r="O19" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="P19" s="17" t="s">
+      <c r="P19" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="Q19" s="16">
+      <c r="Q19" s="18">
         <v>240</v>
       </c>
-      <c r="R19" s="16">
+      <c r="R19" s="23">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K20" s="16">
+      <c r="S19" s="28">
+        <v>0.9</v>
+      </c>
+      <c r="T19" s="26"/>
+    </row>
+    <row r="20" spans="11:20" x14ac:dyDescent="0.25">
+      <c r="K20" s="13">
         <v>12</v>
       </c>
-      <c r="L20" s="16" t="s">
+      <c r="L20" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="M20" s="16"/>
-      <c r="N20" s="17" t="s">
+      <c r="M20" s="13"/>
+      <c r="N20" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="O20" s="17" t="s">
+      <c r="O20" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="P20" s="17" t="s">
+      <c r="P20" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="Q20" s="16">
+      <c r="Q20" s="13">
         <v>60</v>
       </c>
-      <c r="R20" s="16">
+      <c r="R20" s="24">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K21" s="16">
+      <c r="S20" s="28">
+        <v>0</v>
+      </c>
+      <c r="T20" s="29"/>
+    </row>
+    <row r="21" spans="11:20" x14ac:dyDescent="0.25">
+      <c r="K21" s="13">
         <v>13</v>
       </c>
-      <c r="L21" s="16" t="s">
+      <c r="L21" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="M21" s="16"/>
-      <c r="N21" s="17" t="s">
+      <c r="M21" s="13"/>
+      <c r="N21" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="O21" s="17" t="s">
+      <c r="O21" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="P21" s="17" t="s">
+      <c r="P21" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="Q21" s="16">
+      <c r="Q21" s="13">
         <v>60</v>
       </c>
-      <c r="R21" s="16">
+      <c r="R21" s="24">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K22" s="16">
+      <c r="S21" s="28">
+        <v>0</v>
+      </c>
+      <c r="T21" s="29"/>
+    </row>
+    <row r="22" spans="11:20" x14ac:dyDescent="0.25">
+      <c r="K22" s="13">
         <v>14</v>
       </c>
-      <c r="L22" s="16" t="s">
+      <c r="L22" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M22" s="16"/>
-      <c r="N22" s="17" t="s">
+      <c r="M22" s="13"/>
+      <c r="N22" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="O22" s="17" t="s">
+      <c r="O22" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="P22" s="17" t="s">
+      <c r="P22" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="Q22" s="16">
+      <c r="Q22" s="13">
         <v>120</v>
       </c>
-      <c r="R22" s="16">
+      <c r="R22" s="24">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K23" s="16">
+      <c r="S22" s="28">
+        <v>0</v>
+      </c>
+      <c r="T22" s="29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="11:20" x14ac:dyDescent="0.25">
+      <c r="K23" s="13">
         <v>15</v>
       </c>
-      <c r="L23" s="16" t="s">
+      <c r="L23" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="M23" s="16"/>
-      <c r="N23" s="16">
+      <c r="M23" s="13"/>
+      <c r="N23" s="13">
         <v>2</v>
       </c>
-      <c r="O23" s="17" t="s">
+      <c r="O23" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="P23" s="17" t="s">
+      <c r="P23" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="Q23" s="16">
+      <c r="Q23" s="13">
         <v>30</v>
       </c>
-      <c r="R23" s="16">
+      <c r="R23" s="24">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K24" s="16">
+      <c r="S23" s="28">
+        <v>0</v>
+      </c>
+      <c r="T23" s="29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="11:20" x14ac:dyDescent="0.25">
+      <c r="K24" s="13">
         <v>16</v>
       </c>
-      <c r="L24" s="16" t="s">
+      <c r="L24" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="M24" s="16"/>
-      <c r="N24" s="16">
+      <c r="M24" s="13"/>
+      <c r="N24" s="13">
         <v>2</v>
       </c>
-      <c r="O24" s="17" t="s">
+      <c r="O24" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="P24" s="17" t="s">
+      <c r="P24" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="Q24" s="16">
+      <c r="Q24" s="13">
         <v>120</v>
       </c>
-      <c r="R24" s="16">
+      <c r="R24" s="24">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K25" s="16">
+      <c r="S24" s="28">
+        <v>0</v>
+      </c>
+      <c r="T24" s="29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="11:20" x14ac:dyDescent="0.25">
+      <c r="K25" s="13">
         <v>17</v>
       </c>
-      <c r="L25" s="16" t="s">
+      <c r="L25" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="M25" s="16"/>
-      <c r="N25" s="17" t="s">
+      <c r="M25" s="13"/>
+      <c r="N25" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="O25" s="17" t="s">
+      <c r="O25" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="P25" s="17" t="s">
+      <c r="P25" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="Q25" s="16">
+      <c r="Q25" s="13">
         <v>160</v>
       </c>
-      <c r="R25" s="16">
+      <c r="R25" s="24">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K26" s="16">
+      <c r="S25" s="28">
+        <v>0</v>
+      </c>
+      <c r="T25" s="29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="11:20" x14ac:dyDescent="0.25">
+      <c r="K26" s="13">
         <v>18</v>
       </c>
-      <c r="L26" s="18" t="s">
+      <c r="L26" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="M26" s="17"/>
-      <c r="N26" s="17" t="s">
+      <c r="M26" s="14"/>
+      <c r="N26" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="O26" s="17" t="s">
+      <c r="O26" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="P26" s="17" t="s">
+      <c r="P26" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="Q26" s="17">
+      <c r="Q26" s="14">
         <v>30</v>
       </c>
-      <c r="R26" s="17">
+      <c r="R26" s="25">
         <v>3</v>
+      </c>
+      <c r="S26" s="28">
+        <v>0</v>
+      </c>
+      <c r="T26" s="29" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>